<commit_message>
Penambahan dan Rekonfigurasi API, Model, Helper, API Catalogue, Table, dan Stored Procedure
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>date</t>
   </si>
@@ -111,12 +111,20 @@
   <si>
     <t>"additionalProperties": false</t>
   </si>
+  <si>
+    <t>"type": [ "integer", "string" ],
+"minimum": 1,
+"minLength": 1</t>
+  </si>
+  <si>
+    <t>MIXED</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +145,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -195,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -210,6 +225,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -516,13 +534,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E11"/>
+  <dimension ref="B1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -624,17 +642,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+    <row r="10" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Pertanggal 2 Maret 2022 17:46
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -142,6 +142,13 @@
 "pattern": "^((([0-9]{1,4})((-){1})(0[1-9]|1[0-2])((-){1})(0[1-9]|1[0-9]|2[0-9]|3[0-1]))(([ ]{1,})(([0-9]|0[0-9]|1[0-9]|2[0-3]):([0-9]|[0-5][0-9]):([0-9]|[0-5][0-9]))(([.]{1}[0-9]{1,6}){0,1})((([ ]{0,})([+|-]{1})(([0-9]|0[0-9]|1[0-5]){1})){0,1})){0,1})$",
 "minLength": 10,
 "maxLength": 30</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>"type": [ "number", "null" ],
+"minimum": 1</t>
   </si>
 </sst>
 </file>
@@ -558,13 +565,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E13"/>
+  <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -642,65 +649,75 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+    <row r="11" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+    <row r="12" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Pertanggal 9 Maret 2022 17:01
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -568,10 +568,10 @@
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Pertanggal 21 Maret 2022 15:03
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -148,7 +148,7 @@
   </si>
   <si>
     <t>"type": [ "number", "null" ],
-"minimum": 1</t>
+"minimum": 0</t>
   </si>
 </sst>
 </file>
@@ -568,10 +568,10 @@
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Pertanggal 14 Juni 2022 10:08
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -156,18 +156,20 @@
   <si>
     <t>"type": [ "string" ],
 "format": "string",
-"pattern": "^([{]([0-9]{0,})(([,][0-9]{1,}){0,})[}])$",
+"pattern": "^([{]\\s*([0-9]{0,})((\\s*[,]\\s*[0-9]{1,}){0,})\\s*[}])$",
 "minLength": 2</t>
   </si>
   <si>
     <t>{}
 {123}
-{123,456,789}</t>
+{123,456,789}
+{ 123 , 456 , 789 }</t>
   </si>
   <si>
     <t>2
 5
-13</t>
+13
+19</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Update Pertanggal 5 Agustus 2022 19:33 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>date</t>
   </si>
@@ -170,6 +170,18 @@
 5
 13
 19</t>
+  </si>
+  <si>
+    <t>[]
+[123]
+[123,456,789]
+[ 123 , 456 , 789 ]</t>
+  </si>
+  <si>
+    <t>"type": "array",
+"items": {
+    "type": "number"
+    }</t>
   </si>
 </sst>
 </file>
@@ -586,13 +598,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -654,105 +666,115 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
+    <row r="6" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+    <row r="13" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+    <row r="14" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Pertanggal 14 Oktober 2022 11:29  WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>date</t>
   </si>
@@ -182,6 +182,9 @@
 "items": {
     "type": "number"
     }</t>
+  </si>
+  <si>
+    <t>AnyOf</t>
   </si>
 </sst>
 </file>
@@ -598,13 +601,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E16"/>
+  <dimension ref="B1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -776,6 +779,11 @@
       </c>
       <c r="E16" s="5"/>
     </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 28 Desember 2022 18:19 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>date</t>
   </si>
@@ -604,10 +604,10 @@
   <dimension ref="B1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -670,7 +670,9 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C6" s="4" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Update Pertanggal 28 Februari 2023 18:39 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>date</t>
   </si>
@@ -185,6 +185,14 @@
   </si>
   <si>
     <t>AnyOf</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>"type": [ "string" ],
+"format": "string",
+"pattern": "^(([{](((\"[a-zA-Z0-9]{1,}\":((null)|(([0-9]{1,})((.)([0-9]{1,})){0,1})|(\".{1,}\")|([[].*[]])|([{]\"[a-zA-Z0-9]{1,}\":(.*)[}]))),){0,}(\"[a-zA-Z0-9]{1,}\":((null)|([0-9]{1,})|(\"[a-zA-Z0-9]{1,}\")|([[].*[]])|([{]\"[a-zA-Z0-9]{1,}\":(.*)[}]))){0,})[}])|([[]((((null)|(([0-9]{1,})((.)([0-9]{1,})){0,1})|(\".{1,}\")|([[].*[]])|([{]\"[a-zA-Z0-9]{1,}\":(.*)[}])),){0,}((null)|(([0-9]{1,})((.)([0-9]{1,})){0,1})|(\".{1,}\")|([[].*[]])|([{]\"[a-zA-Z0-9]{1,}\":(.*)[}])))[]]))$"</t>
   </si>
 </sst>
 </file>
@@ -601,13 +609,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E18"/>
+  <dimension ref="B1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -691,98 +699,108 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="51" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+    <row r="15" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Pertanggal 2 Maret 2023 12:44 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Restriction" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -612,7 +612,7 @@
   <dimension ref="B1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="C9" sqref="C9"/>

</xml_diff>

<commit_message>
Update Pertanggal 6 Maret 2023 14:35 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>date</t>
   </si>
@@ -193,6 +193,12 @@
     <t>"type": [ "string" ],
 "format": "string",
 "pattern": "^(([{](((\"[a-zA-Z0-9]{1,}\":((null)|(([0-9]{1,})((.)([0-9]{1,})){0,1})|(\".{1,}\")|([[].*[]])|([{]\"[a-zA-Z0-9]{1,}\":(.*)[}]))),){0,}(\"[a-zA-Z0-9]{1,}\":((null)|([0-9]{1,})|(\"[a-zA-Z0-9]{1,}\")|([[].*[]])|([{]\"[a-zA-Z0-9]{1,}\":(.*)[}]))){0,})[}])|([[]((((null)|(([0-9]{1,})((.)([0-9]{1,})){0,1})|(\".{1,}\")|([[].*[]])|([{]\"[a-zA-Z0-9]{1,}\":(.*)[}])),){0,}((null)|(([0-9]{1,})((.)([0-9]{1,})){0,1})|(\".{1,}\")|([[].*[]])|([{]\"[a-zA-Z0-9]{1,}\":(.*)[}])))[]]))$"</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>"type": "boolean"</t>
   </si>
 </sst>
 </file>
@@ -609,13 +615,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E19"/>
+  <dimension ref="B1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -711,96 +717,106 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="2:5" ht="51" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+    <row r="15" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+    <row r="16" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Pertanggal 14 Agustus 2023 13:56 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -618,10 +618,10 @@
   <dimension ref="B1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Pertanggal 8 Januari 2025 19:00 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>date</t>
   </si>
@@ -199,6 +199,24 @@
   </si>
   <si>
     <t>"type": "boolean"</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>"type": [ "string", "null" ],
+"format": "string",
+"pattern": "^(([ ]{0,})([(]{0,1})([ ]{0,})(([+]{0,1}|[-]{0,1}){0,1})((([0-8]{0,1})([0-9]{0,1})([.])([0-9]{0,7}))|((90)((([.])([0]{0,7})){0,1})))([ ]{0,})([,])([ ]{0,})(([+]{0,1}|[-]{0,1}){0,1})((((([0-9])|([1-9][0-9])|(1([0-7][0-9]))){0,1})((([.])([0-9]{0,7})){0,1}))|((180)((([.])([0]{0,7})){0,1})))([ ]{0,})([)]{0,1})([ ]{0,}))$",
+"minLength": 1,
+"maxLength": 27</t>
+  </si>
+  <si>
+    <t>90.0000000, 180.0000000
++90.0000000, +180.0000000
++90.0000000, -180.0000000
+(-90.0000000, +180.0000000)
+.1234567, .2345678
+(+.1234567, -.2345678)</t>
   </si>
 </sst>
 </file>
@@ -615,13 +633,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E20"/>
+  <dimension ref="B1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -765,58 +783,70 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="2:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+    <row r="16" spans="2:5" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+    <row r="17" spans="2:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. Penambahan API    dataPickList.humanResource.getPersonBusinessTripSequenceDetail dan transaction.read.dataList.humanResource.getPersonBusinessTripSequenceDetail 2. Homogenisasi Respon API transaction.read.dataList
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/JSON Schema Restriction.xlsx
@@ -636,10 +636,10 @@
   <dimension ref="B1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>